<commit_message>
24/5/25 3 lecture DSA LB
</commit_message>
<xml_diff>
--- a/Excel/DSA_CTCI_Tracker.xlsx
+++ b/Excel/DSA_CTCI_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ghanu Study\Varnagi Learning\Languages\DSA\DSA_LB-Own\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2B27BA-1093-4560-B979-2D41EDA62613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CEC5FD-2B52-47F5-B108-B7B3A46C8AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,14 +399,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -715,7 +714,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,7 +732,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -759,410 +758,565 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" t="s">
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G3" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G4" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G5" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G6" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G7" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G8" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G9" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G10" t="s">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G11" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
         <v>74</v>
       </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G12" t="s">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G13" t="s">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G14" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G15" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G16" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G17" t="s">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G18" t="s">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G19" t="s">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G20" t="s">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G21" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G22" t="s">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G23" t="s">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D24" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G24" t="s">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G25" t="s">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G26" t="s">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D27" t="s">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G27" t="s">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G28" t="s">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G29" t="s">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D30" t="s">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G30" t="s">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
till binary search in nearly sorted array
</commit_message>
<xml_diff>
--- a/Excel/DSA_CTCI_Tracker.xlsx
+++ b/Excel/DSA_CTCI_Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ghanu Study\Varnagi Learning\Languages\DSA\DSA_LB-Own\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AF4457-F2F3-46F0-9E79-A8A03202BE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C141ECE8-0C07-4140-9BFC-93E1654ED345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -379,12 +379,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -414,12 +420,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -729,7 +738,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,7 +789,7 @@
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C2" s="2">
@@ -810,7 +819,7 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C3" s="2">
@@ -842,7 +851,7 @@
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C4" s="2">
@@ -874,7 +883,7 @@
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C5" s="2">
@@ -906,7 +915,7 @@
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C6" s="2"/>
@@ -926,7 +935,7 @@
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C7" s="2"/>
@@ -946,7 +955,7 @@
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C8" s="2"/>
@@ -966,7 +975,7 @@
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C9" s="2"/>
@@ -986,7 +995,7 @@
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C10" s="2"/>
@@ -1006,7 +1015,7 @@
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C11" s="2"/>
@@ -1026,7 +1035,7 @@
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>87</v>
       </c>
       <c r="C12" s="2"/>
@@ -1046,7 +1055,7 @@
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C13" s="2"/>
@@ -1066,7 +1075,7 @@
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C14" s="2"/>

</xml_diff>